<commit_message>
update lab2 to exp3
</commit_message>
<xml_diff>
--- a/lab1/4dk4 lab1/lab1 excel.xlsx
+++ b/lab1/4dk4 lab1/lab1 excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardqiu/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardqiu/Desktop/Computer_Network/lab1/4dk4 lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{546E73E1-6679-3F42-8114-296FF7ED4127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112A3601-DED3-374A-9F0E-320A75842654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="2200" windowWidth="38400" windowHeight="21100" xr2:uid="{3DE9DE84-1883-E343-8A9E-104C0733BF92}"/>
   </bookViews>
@@ -16,12 +16,16 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$F$111:$F$120</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$G$111:$G$120</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$F$111:$F$120</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$G$111:$G$120</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$D$19:$D$28</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$D$3:$D$12</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$E$19:$E$28</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$E$3:$E$12</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$19:$D$28</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$3:$D$12</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$E$19:$E$28</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$3:$E$12</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -7083,8 +7087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D60337A-CE44-1241-9789-2441B98310D3}">
   <dimension ref="C2:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O95" sqref="O95"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="151" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7137,7 +7141,7 @@
         <v>5.5866910000000001</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F28" si="0">C4*(2-D4*C4)/(2*(1-C4*D4))</f>
+        <f t="shared" ref="F4:F27" si="0">C4*(2-D4*C4)/(2*(1-C4*D4))</f>
         <v>5.5864197530864201</v>
       </c>
     </row>

</xml_diff>